<commit_message>
Actualizacion cronograma semana 8
</commit_message>
<xml_diff>
--- a/Cronograma de actividades Sistemas Operativos.xlsx
+++ b/Cronograma de actividades Sistemas Operativos.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geovani\Documents\CURSOS_2020_SEMESTRE2\SISTEMAS OPERATIVOS 1\Cronograma\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>No. Actividad</t>
   </si>
@@ -148,12 +153,18 @@
   </si>
   <si>
     <t>Interrupciones E/S</t>
+  </si>
+  <si>
+    <t>Parte Inicial</t>
+  </si>
+  <si>
+    <t>Parte Final</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -242,7 +253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -277,19 +288,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -353,7 +367,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -388,7 +402,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -565,7 +579,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -575,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E4:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,40 +604,40 @@
   </cols>
   <sheetData>
     <row r="4" spans="5:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="8" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="16" t="s">
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="16"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
     </row>
     <row r="9" spans="5:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="J9" s="20" t="s">
+      <c r="J9" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -665,7 +679,7 @@
         <v>8</v>
       </c>
       <c r="J11" s="9">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="5:10" x14ac:dyDescent="0.25">
@@ -684,7 +698,7 @@
         <v>8</v>
       </c>
       <c r="J12" s="9">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="5:10" x14ac:dyDescent="0.25">
@@ -705,7 +719,7 @@
         <v>12</v>
       </c>
       <c r="J13" s="9">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="5:10" x14ac:dyDescent="0.25">
@@ -726,7 +740,7 @@
         <v>14</v>
       </c>
       <c r="J14" s="9">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="5:10" x14ac:dyDescent="0.25">
@@ -747,7 +761,7 @@
         <v>16</v>
       </c>
       <c r="J15" s="9">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="5:10" x14ac:dyDescent="0.25">
@@ -781,7 +795,7 @@
         <v>Geovani</v>
       </c>
       <c r="J17" s="9">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="18" spans="5:10" x14ac:dyDescent="0.25">
@@ -802,7 +816,7 @@
         <v>Angel</v>
       </c>
       <c r="J18" s="9">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="19" spans="5:10" x14ac:dyDescent="0.25">
@@ -822,7 +836,7 @@
         <v>14</v>
       </c>
       <c r="J19" s="9">
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="20" spans="5:10" x14ac:dyDescent="0.25">
@@ -842,7 +856,7 @@
         <v>16</v>
       </c>
       <c r="J20" s="9">
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="21" spans="5:10" x14ac:dyDescent="0.25">
@@ -895,7 +909,7 @@
         <v>21</v>
       </c>
       <c r="J23" s="9">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="5:10" x14ac:dyDescent="0.25">
@@ -913,10 +927,10 @@
         <v>44094</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J24" s="9">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="25" spans="5:10" x14ac:dyDescent="0.25">
@@ -937,7 +951,7 @@
         <v>28</v>
       </c>
       <c r="J25" s="9">
-        <v>0</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="26" spans="5:10" x14ac:dyDescent="0.25">
@@ -955,10 +969,10 @@
         <v>44094</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J26" s="9">
-        <v>0</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="27" spans="5:10" x14ac:dyDescent="0.25">
@@ -1055,7 +1069,7 @@
     </row>
     <row r="32" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E32" s="14">
-        <f t="shared" ref="E32:E34" si="2">E31+0.1</f>
+        <f t="shared" ref="E32:E33" si="2">E31+0.1</f>
         <v>9.1999999999999993</v>
       </c>
       <c r="F32" s="13" t="s">
@@ -1097,40 +1111,56 @@
     </row>
     <row r="34" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E34" s="14">
-        <f t="shared" si="2"/>
+        <f>E33+0.1</f>
         <v>9.3999999999999986</v>
       </c>
       <c r="F34" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G34" s="7">
+      <c r="I34" s="14"/>
+      <c r="J34" s="9"/>
+    </row>
+    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E35" s="16">
+        <f t="shared" ref="E35:E36" si="3">E34+0.1</f>
+        <v>9.4999999999999982</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G35" s="7">
         <v>44085</v>
       </c>
-      <c r="H34" s="6">
+      <c r="H35" s="6">
         <v>44090</v>
       </c>
-      <c r="I34" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J34" s="9">
+      <c r="I35" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E35" s="14"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="9"/>
-    </row>
     <row r="36" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E36" s="14"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="9"/>
+      <c r="E36" s="16">
+        <f t="shared" si="3"/>
+        <v>9.5999999999999979</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G36" s="7">
+        <v>44085</v>
+      </c>
+      <c r="H36" s="6">
+        <v>44090</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J36" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E37" s="14">
@@ -1162,12 +1192,12 @@
         <v>21</v>
       </c>
       <c r="J38" s="9">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="39" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E39" s="14">
-        <f t="shared" ref="E39:E40" si="3">E38+0.1</f>
+        <f t="shared" ref="E39:E40" si="4">E38+0.1</f>
         <v>10.199999999999999</v>
       </c>
       <c r="F39" s="5" t="s">
@@ -1188,7 +1218,7 @@
     </row>
     <row r="40" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E40" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10.299999999999999</v>
       </c>
       <c r="F40" s="5" t="s">

</xml_diff>